<commit_message>
Adding modified 'Z Axis Bearing Cup Top' to give clearance for router and stop it hitting the upper Z limit tab
</commit_message>
<xml_diff>
--- a/BOM/R3 BOM.xlsx
+++ b/BOM/R3 BOM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MACHINE\Google Drive\CNC_pete\Rev 1.3\STL\R3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tschubb\Documents\Root-3-CNC\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1682037-64C2-46C4-ADAA-078F05F03C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17895" windowHeight="7965" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="32220" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3D Printed Parts" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="163">
   <si>
     <t>Item</t>
   </si>
@@ -509,12 +510,18 @@
   </si>
   <si>
     <t>5/7</t>
+  </si>
+  <si>
+    <t>Z Axis Bearing Cup Top - Limit Tab Removed</t>
+  </si>
+  <si>
+    <t>Allows clearance for router (Makita in my case) by removing the upper Z limit switch tab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -766,7 +773,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="11">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -846,6 +853,20 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -860,46 +881,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table135" displayName="Table135" ref="A1:H58" totalsRowShown="0">
-  <autoFilter ref="A1:H58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table135" displayName="Table135" ref="A1:H59" totalsRowShown="0">
+  <autoFilter ref="A1:H59" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Item" dataDxfId="6"/>
-    <tableColumn id="2" name="QTY"/>
-    <tableColumn id="3" name="Printed"/>
-    <tableColumn id="5" name="Config"/>
-    <tableColumn id="6" name="Stepper Config"/>
-    <tableColumn id="7" name="1&quot; or 25mm Box"/>
-    <tableColumn id="8" name="Belt Size"/>
-    <tableColumn id="4" name="Notes"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="QTY"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Printed"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Config"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Stepper Config"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="1&quot; or 25mm Box"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Belt Size"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:G32" totalsRowShown="0" headerRowBorderDxfId="5">
-  <autoFilter ref="A1:G32"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:G32" totalsRowShown="0" headerRowBorderDxfId="5">
+  <autoFilter ref="A1:G32" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Item" dataDxfId="4"/>
-    <tableColumn id="2" name="QTY" dataDxfId="3"/>
-    <tableColumn id="4" name="Config"/>
-    <tableColumn id="5" name="Stepper Config"/>
-    <tableColumn id="6" name="1&quot; or 25mm Box"/>
-    <tableColumn id="7" name="Belt Size"/>
-    <tableColumn id="8" name="Notes"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Item" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="QTY" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Config"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Stepper Config"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="1&quot; or 25mm Box"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Belt Size"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="A1:D29" totalsRowShown="0">
-  <autoFilter ref="A1:D29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:D29" totalsRowShown="0">
+  <autoFilter ref="A1:D29" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Item" dataDxfId="0"/>
-    <tableColumn id="2" name="QTY"/>
-    <tableColumn id="4" name="Ordered?"/>
-    <tableColumn id="3" name="Notes"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Item" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="QTY"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Ordered?"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1201,26 +1222,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H58"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="A1:H2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="40.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="78.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="78.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>50</v>
       </c>
@@ -1270,7 +1291,7 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>117</v>
       </c>
@@ -1284,7 +1305,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>51</v>
       </c>
@@ -1308,7 +1329,7 @@
       </c>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="21" t="s">
         <v>52</v>
       </c>
@@ -1332,7 +1353,7 @@
       </c>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="20" t="s">
         <v>58</v>
       </c>
@@ -1346,7 +1367,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>59</v>
       </c>
@@ -1370,7 +1391,7 @@
       </c>
       <c r="H7" s="10"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>116</v>
       </c>
@@ -1382,7 +1403,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>60</v>
       </c>
@@ -1406,7 +1427,7 @@
       </c>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>61</v>
       </c>
@@ -1430,7 +1451,7 @@
       </c>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>74</v>
       </c>
@@ -1454,7 +1475,7 @@
       </c>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>75</v>
       </c>
@@ -1478,7 +1499,7 @@
       </c>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>115</v>
       </c>
@@ -1490,7 +1511,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>62</v>
       </c>
@@ -1514,7 +1535,7 @@
       </c>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>63</v>
       </c>
@@ -1538,7 +1559,7 @@
       </c>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>76</v>
       </c>
@@ -1562,7 +1583,7 @@
       </c>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="14" t="s">
         <v>77</v>
       </c>
@@ -1586,7 +1607,7 @@
       </c>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="19" t="s">
         <v>65</v>
       </c>
@@ -1600,7 +1621,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>67</v>
       </c>
@@ -1624,7 +1645,7 @@
       </c>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>116</v>
       </c>
@@ -1636,7 +1657,7 @@
       <c r="G20" s="9"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>68</v>
       </c>
@@ -1660,7 +1681,7 @@
       </c>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="14" t="s">
         <v>69</v>
       </c>
@@ -1684,7 +1705,7 @@
       </c>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
         <v>74</v>
       </c>
@@ -1708,7 +1729,7 @@
       </c>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="14" t="s">
         <v>75</v>
       </c>
@@ -1732,7 +1753,7 @@
       </c>
       <c r="H24" s="10"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="14" t="s">
         <v>115</v>
       </c>
@@ -1744,7 +1765,7 @@
       <c r="G25" s="9"/>
       <c r="H25" s="10"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="14" t="s">
         <v>70</v>
       </c>
@@ -1768,7 +1789,7 @@
       </c>
       <c r="H26" s="10"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="14" t="s">
         <v>71</v>
       </c>
@@ -1792,7 +1813,7 @@
       </c>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="14" t="s">
         <v>76</v>
       </c>
@@ -1816,7 +1837,7 @@
       </c>
       <c r="H28" s="10"/>
     </row>
-    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="15" t="s">
         <v>77</v>
       </c>
@@ -1840,7 +1861,7 @@
       </c>
       <c r="H29" s="12"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="s">
         <v>72</v>
       </c>
@@ -1864,7 +1885,7 @@
       </c>
       <c r="H30" s="8"/>
     </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="22" t="s">
         <v>79</v>
       </c>
@@ -1888,7 +1909,7 @@
       </c>
       <c r="H31" s="24"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
         <v>73</v>
       </c>
@@ -1912,7 +1933,7 @@
       </c>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="15" t="s">
         <v>80</v>
       </c>
@@ -1936,7 +1957,7 @@
       </c>
       <c r="H33" s="12"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>78</v>
       </c>
@@ -1959,7 +1980,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>81</v>
       </c>
@@ -1985,7 +2006,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
         <v>83</v>
       </c>
@@ -2009,7 +2030,7 @@
       </c>
       <c r="H36" s="8"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>118</v>
       </c>
@@ -2033,7 +2054,7 @@
       </c>
       <c r="H37" s="10"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
         <v>117</v>
       </c>
@@ -2047,7 +2068,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
         <v>84</v>
       </c>
@@ -2071,7 +2092,7 @@
       </c>
       <c r="H39" s="10"/>
     </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="21" t="s">
         <v>85</v>
       </c>
@@ -2095,7 +2116,7 @@
       </c>
       <c r="H40" s="12"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>87</v>
       </c>
@@ -2118,7 +2139,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>88</v>
       </c>
@@ -2141,7 +2162,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>89</v>
       </c>
@@ -2164,7 +2185,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>90</v>
       </c>
@@ -2187,12 +2208,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>92</v>
       </c>
@@ -2215,7 +2236,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>93</v>
       </c>
@@ -2238,192 +2259,195 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
+    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" t="s">
+        <v>105</v>
+      </c>
+      <c r="F48" t="s">
+        <v>105</v>
+      </c>
+      <c r="G48" t="s">
+        <v>105</v>
+      </c>
+      <c r="H48" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="8"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="8"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="B49" s="9">
+      <c r="B50" s="9">
         <v>1</v>
       </c>
-      <c r="C49" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D49" s="9" t="s">
+      <c r="C50" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E49" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G49" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H49" s="10"/>
-    </row>
-    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="22" t="s">
+      <c r="E50" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H50" s="10"/>
+    </row>
+    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A51" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B50" s="23">
+      <c r="B51" s="23">
         <v>1</v>
       </c>
-      <c r="C50" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D50" s="23" t="s">
+      <c r="C51" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="E50" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="F50" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="G50" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="H50" s="24"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
+      <c r="E51" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F51" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="G51" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="H51" s="24"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="B51" s="9">
+      <c r="B52" s="9">
         <v>1</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F51" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H51" s="10" t="s">
+      <c r="C52" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H52" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="22" t="s">
+    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="B52" s="23">
+      <c r="B53" s="23">
         <v>1</v>
       </c>
-      <c r="C52" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D52" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E52" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="F52" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="G52" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="H52" s="24" t="s">
+      <c r="C53" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="F53" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="G53" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="H53" s="24" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="B53" s="9">
+      <c r="B54" s="9">
         <v>1</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D53" s="9" t="s">
+      <c r="C54" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D54" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E53" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F53" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="H53" s="10"/>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="15" t="s">
+      <c r="E54" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="H54" s="10"/>
+    </row>
+    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A55" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B55" s="11">
         <v>1</v>
       </c>
-      <c r="C54" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D54" s="11" t="s">
+      <c r="C55" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D55" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E54" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="F54" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="G54" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H54" s="12"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="E55" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H55" s="12"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55" t="s">
-        <v>36</v>
-      </c>
-      <c r="D55" t="s">
-        <v>55</v>
-      </c>
-      <c r="E55" t="s">
-        <v>105</v>
-      </c>
-      <c r="F55" t="s">
-        <v>105</v>
-      </c>
-      <c r="G55" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -2444,9 +2468,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -2467,9 +2491,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -2490,29 +2514,60 @@
         <v>105</v>
       </c>
     </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>36</v>
+      </c>
+      <c r="D59" t="s">
+        <v>55</v>
+      </c>
+      <c r="E59" t="s">
+        <v>105</v>
+      </c>
+      <c r="F59" t="s">
+        <v>105</v>
+      </c>
+      <c r="G59" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C58">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+  <conditionalFormatting sqref="C2:C47 C49:C59">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C48">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C59" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D59" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Default,Optional"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E59" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"N/A, NEMA17,NEMA23"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F59" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"N/A,1"",25mm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G59" xr:uid="{00000000-0002-0000-0000-000004000000}">
       <formula1>"N/A,GT2 (2mm), 3M HTD (3mm)"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2524,25 +2579,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="55.42578125" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.453125" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="60.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="60.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
@@ -2569,7 +2624,7 @@
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>123</v>
       </c>
@@ -2586,7 +2641,7 @@
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="26" t="s">
         <v>124</v>
       </c>
@@ -2605,7 +2660,7 @@
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
         <v>126</v>
       </c>
@@ -2622,7 +2677,7 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>127</v>
       </c>
@@ -2641,7 +2696,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
         <v>122</v>
       </c>
@@ -2666,7 +2721,7 @@
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="25" t="s">
         <v>120</v>
       </c>
@@ -2683,7 +2738,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>121</v>
       </c>
@@ -2700,7 +2755,7 @@
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="25" t="s">
         <v>125</v>
       </c>
@@ -2717,7 +2772,7 @@
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>156</v>
       </c>
@@ -2738,7 +2793,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="25" t="s">
         <v>129</v>
       </c>
@@ -2755,7 +2810,7 @@
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>130</v>
       </c>
@@ -2774,7 +2829,7 @@
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
         <v>131</v>
       </c>
@@ -2793,7 +2848,7 @@
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>134</v>
       </c>
@@ -2812,7 +2867,7 @@
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="25" t="s">
         <v>145</v>
       </c>
@@ -2829,7 +2884,7 @@
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>132</v>
       </c>
@@ -2848,7 +2903,7 @@
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="25" t="s">
         <v>133</v>
       </c>
@@ -2867,7 +2922,7 @@
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="25" t="s">
         <v>135</v>
       </c>
@@ -2884,7 +2939,7 @@
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" s="25" t="s">
         <v>136</v>
       </c>
@@ -2901,7 +2956,7 @@
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
         <v>143</v>
       </c>
@@ -2918,7 +2973,7 @@
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="25" t="s">
         <v>146</v>
       </c>
@@ -2937,7 +2992,7 @@
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
         <v>137</v>
       </c>
@@ -2954,7 +3009,7 @@
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" s="25" t="s">
         <v>138</v>
       </c>
@@ -2971,7 +3026,7 @@
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
         <v>139</v>
       </c>
@@ -2990,7 +3045,7 @@
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="25" t="s">
         <v>140</v>
       </c>
@@ -3009,7 +3064,7 @@
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="25" t="s">
         <v>141</v>
       </c>
@@ -3028,7 +3083,7 @@
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" s="25" t="s">
         <v>153</v>
       </c>
@@ -3049,7 +3104,7 @@
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="25" t="s">
         <v>144</v>
       </c>
@@ -3066,7 +3121,7 @@
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" s="25" t="s">
         <v>155</v>
       </c>
@@ -3083,7 +3138,7 @@
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>157</v>
       </c>
@@ -3104,7 +3159,7 @@
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>158</v>
       </c>
@@ -3125,7 +3180,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="25"/>
       <c r="B32" s="28"/>
       <c r="C32" s="9"/>
@@ -3138,7 +3193,7 @@
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
       <c r="B33" s="28"/>
       <c r="C33" s="9"/>
@@ -3151,7 +3206,7 @@
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
       <c r="B34" s="28"/>
       <c r="C34" s="9"/>
@@ -3164,7 +3219,7 @@
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
       <c r="B35" s="28"/>
       <c r="C35" s="9"/>
@@ -3179,16 +3234,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F32" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"N/A,GT2 (2mm), 3M HTD (3mm)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E32" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"N/A,1"",25mm"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D32" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"N/A, NEMA17,NEMA23"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C32" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"Default,Optional"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3201,21 +3256,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="134" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3229,7 +3284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -3240,7 +3295,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -3251,7 +3306,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -3262,7 +3317,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -3273,7 +3328,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -3284,7 +3339,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -3295,7 +3350,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
@@ -3303,7 +3358,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -3314,7 +3369,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
@@ -3322,7 +3377,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -3333,7 +3388,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -3344,7 +3399,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -3352,7 +3407,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -3363,7 +3418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>5</v>
       </c>
@@ -3374,7 +3429,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -3385,7 +3440,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -3396,7 +3451,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
@@ -3407,7 +3462,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -3418,7 +3473,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -3429,7 +3484,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -3440,7 +3495,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
@@ -3451,7 +3506,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
@@ -3459,7 +3514,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>31</v>
       </c>
@@ -3470,7 +3525,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>33</v>
       </c>
@@ -3481,7 +3536,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>37</v>
       </c>
@@ -3492,7 +3547,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
@@ -3503,7 +3558,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
@@ -3514,7 +3569,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -3535,7 +3590,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C29" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>